<commit_message>
Mise en conformité pour 2024-2025
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -1,28 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\Cours\BAC-3 -  Projet individuel\22-23\template-github\agenda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\Cours\INFOB318  - Projet individuel\INFOB318-template\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285C76F8-B471-48E9-8EBF-C2BF505744E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15000" windowHeight="7830"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="effort" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t>…</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Total/Semaine</t>
   </si>
@@ -47,11 +58,23 @@
   <si>
     <t>Total:</t>
   </si>
+  <si>
+    <t>Tampon de récupération (dodo)</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Rencontres</t>
+  </si>
+  <si>
+    <t>etc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -530,7 +553,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="22" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -568,9 +591,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -608,9 +631,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,7 +668,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,7 +703,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -853,28 +876,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AH46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
-    <col min="4" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-    <col min="11" max="16" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="11" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:34" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
@@ -882,9 +905,9 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" spans="2:34" ht="21" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:34" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -892,9 +915,9 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="2:34" ht="21" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:34" ht="21" x14ac:dyDescent="0.4">
       <c r="B4" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -902,9 +925,9 @@
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
     </row>
-    <row r="5" spans="2:34" ht="21" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:34" ht="21" x14ac:dyDescent="0.4">
       <c r="B5" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -912,10 +935,10 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
     </row>
-    <row r="6" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="19">
         <f>SUM(D11:D36)</f>
@@ -1042,140 +1065,140 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>44823</v>
+        <v>45579</v>
       </c>
       <c r="E8" s="2">
         <f>D8+7</f>
-        <v>44830</v>
+        <v>45586</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:Q8" si="2">E8+7</f>
-        <v>44837</v>
+        <v>45593</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="2"/>
-        <v>44844</v>
+        <v>45600</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>44851</v>
+        <v>45607</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="2"/>
-        <v>44858</v>
+        <v>45614</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="2"/>
-        <v>44865</v>
+        <v>45621</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" si="2"/>
-        <v>44872</v>
+        <v>45628</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="2"/>
-        <v>44879</v>
+        <v>45635</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="2"/>
-        <v>44886</v>
+        <v>45642</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
-        <v>44893</v>
+        <v>45649</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="2"/>
-        <v>44900</v>
+        <v>45656</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="2"/>
-        <v>44907</v>
+        <v>45663</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" si="2"/>
-        <v>44914</v>
+        <v>45670</v>
       </c>
       <c r="R8" s="3">
         <f t="shared" ref="R8" si="3">Q8+7</f>
-        <v>44921</v>
+        <v>45677</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" ref="S8" si="4">R8+7</f>
-        <v>44928</v>
+        <v>45684</v>
       </c>
       <c r="T8" s="3">
         <f t="shared" ref="T8" si="5">S8+7</f>
-        <v>44935</v>
+        <v>45691</v>
       </c>
       <c r="U8" s="3">
         <f t="shared" ref="U8" si="6">T8+7</f>
-        <v>44942</v>
+        <v>45698</v>
       </c>
       <c r="V8" s="3">
         <f t="shared" ref="V8" si="7">U8+7</f>
-        <v>44949</v>
+        <v>45705</v>
       </c>
       <c r="W8" s="3">
         <f t="shared" ref="W8" si="8">V8+7</f>
-        <v>44956</v>
+        <v>45712</v>
       </c>
       <c r="X8" s="3">
         <f t="shared" ref="X8" si="9">W8+7</f>
-        <v>44963</v>
+        <v>45719</v>
       </c>
       <c r="Y8" s="3">
         <f t="shared" ref="Y8" si="10">X8+7</f>
-        <v>44970</v>
+        <v>45726</v>
       </c>
       <c r="Z8" s="3">
         <f t="shared" ref="Z8:AH8" si="11">Y8+7</f>
-        <v>44977</v>
+        <v>45733</v>
       </c>
       <c r="AA8" s="3">
         <f t="shared" si="11"/>
-        <v>44984</v>
+        <v>45740</v>
       </c>
       <c r="AB8" s="3">
         <f t="shared" si="11"/>
-        <v>44991</v>
+        <v>45747</v>
       </c>
       <c r="AC8" s="3">
         <f t="shared" si="11"/>
-        <v>44998</v>
+        <v>45754</v>
       </c>
       <c r="AD8" s="3">
         <f t="shared" si="11"/>
-        <v>45005</v>
+        <v>45761</v>
       </c>
       <c r="AE8" s="3">
         <f t="shared" si="11"/>
-        <v>45012</v>
+        <v>45768</v>
       </c>
       <c r="AF8" s="3">
         <f t="shared" si="11"/>
-        <v>45019</v>
+        <v>45775</v>
       </c>
       <c r="AG8" s="3">
         <f t="shared" si="11"/>
-        <v>45026</v>
+        <v>45782</v>
       </c>
       <c r="AH8" s="3">
         <f t="shared" si="11"/>
-        <v>45033</v>
-      </c>
-    </row>
-    <row r="9" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="22">
         <f>SUM(C10:C46)</f>
@@ -1306,8 +1329,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="27"/>
+    <row r="10" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="27" t="s">
+        <v>8</v>
+      </c>
       <c r="C10" s="25">
         <f>SUM(D10:AH10)</f>
         <v>0</v>
@@ -1344,8 +1369,10 @@
       <c r="AG10" s="11"/>
       <c r="AH10" s="11"/>
     </row>
-    <row r="11" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="7"/>
+    <row r="11" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="C11" s="25">
         <f t="shared" ref="C11:C46" si="14">SUM(D11:AH11)</f>
         <v>0</v>
@@ -1382,8 +1409,10 @@
       <c r="AG11" s="13"/>
       <c r="AH11" s="13"/>
     </row>
-    <row r="12" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="7"/>
+    <row r="12" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="C12" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1420,8 +1449,10 @@
       <c r="AG12" s="13"/>
       <c r="AH12" s="13"/>
     </row>
-    <row r="13" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C13" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1458,7 +1489,7 @@
       <c r="AG13" s="13"/>
       <c r="AH13" s="13"/>
     </row>
-    <row r="14" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
       <c r="C14" s="25">
         <f t="shared" si="14"/>
@@ -1496,7 +1527,7 @@
       <c r="AG14" s="13"/>
       <c r="AH14" s="13"/>
     </row>
-    <row r="15" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="25">
         <f t="shared" si="14"/>
@@ -1534,7 +1565,7 @@
       <c r="AG15" s="13"/>
       <c r="AH15" s="13"/>
     </row>
-    <row r="16" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
       <c r="C16" s="25">
         <f t="shared" si="14"/>
@@ -1572,7 +1603,7 @@
       <c r="AG16" s="13"/>
       <c r="AH16" s="13"/>
     </row>
-    <row r="17" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
       <c r="C17" s="25">
         <f t="shared" si="14"/>
@@ -1610,7 +1641,7 @@
       <c r="AG17" s="13"/>
       <c r="AH17" s="13"/>
     </row>
-    <row r="18" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
       <c r="C18" s="25">
         <f t="shared" si="14"/>
@@ -1648,7 +1679,7 @@
       <c r="AG18" s="13"/>
       <c r="AH18" s="13"/>
     </row>
-    <row r="19" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="25">
         <f t="shared" si="14"/>
@@ -1686,7 +1717,7 @@
       <c r="AG19" s="13"/>
       <c r="AH19" s="13"/>
     </row>
-    <row r="20" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
       <c r="C20" s="25">
         <f t="shared" si="14"/>
@@ -1724,7 +1755,7 @@
       <c r="AG20" s="13"/>
       <c r="AH20" s="13"/>
     </row>
-    <row r="21" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
       <c r="C21" s="25">
         <f t="shared" si="14"/>
@@ -1762,7 +1793,7 @@
       <c r="AG21" s="13"/>
       <c r="AH21" s="13"/>
     </row>
-    <row r="22" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
       <c r="C22" s="25">
         <f t="shared" si="14"/>
@@ -1800,7 +1831,7 @@
       <c r="AG22" s="13"/>
       <c r="AH22" s="13"/>
     </row>
-    <row r="23" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
       <c r="C23" s="25">
         <f t="shared" si="14"/>
@@ -1838,7 +1869,7 @@
       <c r="AG23" s="13"/>
       <c r="AH23" s="13"/>
     </row>
-    <row r="24" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
       <c r="C24" s="25">
         <f t="shared" si="14"/>
@@ -1876,7 +1907,7 @@
       <c r="AG24" s="13"/>
       <c r="AH24" s="13"/>
     </row>
-    <row r="25" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
       <c r="C25" s="25">
         <f t="shared" si="14"/>
@@ -1914,7 +1945,7 @@
       <c r="AG25" s="13"/>
       <c r="AH25" s="13"/>
     </row>
-    <row r="26" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7"/>
       <c r="C26" s="25">
         <f t="shared" si="14"/>
@@ -1952,7 +1983,7 @@
       <c r="AG26" s="13"/>
       <c r="AH26" s="13"/>
     </row>
-    <row r="27" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7"/>
       <c r="C27" s="25">
         <f t="shared" si="14"/>
@@ -1990,7 +2021,7 @@
       <c r="AG27" s="13"/>
       <c r="AH27" s="13"/>
     </row>
-    <row r="28" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="7"/>
       <c r="C28" s="25">
         <f t="shared" si="14"/>
@@ -2028,7 +2059,7 @@
       <c r="AG28" s="13"/>
       <c r="AH28" s="13"/>
     </row>
-    <row r="29" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
       <c r="C29" s="25">
         <f t="shared" si="14"/>
@@ -2066,7 +2097,7 @@
       <c r="AG29" s="13"/>
       <c r="AH29" s="13"/>
     </row>
-    <row r="30" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="7"/>
       <c r="C30" s="25">
         <f t="shared" si="14"/>
@@ -2104,7 +2135,7 @@
       <c r="AG30" s="13"/>
       <c r="AH30" s="13"/>
     </row>
-    <row r="31" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="7"/>
       <c r="C31" s="25">
         <f t="shared" si="14"/>
@@ -2142,7 +2173,7 @@
       <c r="AG31" s="13"/>
       <c r="AH31" s="13"/>
     </row>
-    <row r="32" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="7"/>
       <c r="C32" s="25">
         <f t="shared" si="14"/>
@@ -2180,7 +2211,7 @@
       <c r="AG32" s="13"/>
       <c r="AH32" s="13"/>
     </row>
-    <row r="33" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="7"/>
       <c r="C33" s="25">
         <f t="shared" si="14"/>
@@ -2218,7 +2249,7 @@
       <c r="AG33" s="13"/>
       <c r="AH33" s="13"/>
     </row>
-    <row r="34" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
       <c r="C34" s="25">
         <f t="shared" si="14"/>
@@ -2256,7 +2287,7 @@
       <c r="AG34" s="13"/>
       <c r="AH34" s="13"/>
     </row>
-    <row r="35" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8"/>
       <c r="C35" s="25">
         <f t="shared" si="14"/>
@@ -2294,10 +2325,8 @@
       <c r="AG35" s="13"/>
       <c r="AH35" s="13"/>
     </row>
-    <row r="36" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="7" t="s">
-        <v>0</v>
-      </c>
+    <row r="36" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="7"/>
       <c r="C36" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2334,10 +2363,8 @@
       <c r="AG36" s="13"/>
       <c r="AH36" s="13"/>
     </row>
-    <row r="37" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="7" t="s">
-        <v>0</v>
-      </c>
+    <row r="37" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7"/>
       <c r="C37" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2374,10 +2401,8 @@
       <c r="AG37" s="13"/>
       <c r="AH37" s="13"/>
     </row>
-    <row r="38" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="7" t="s">
-        <v>0</v>
-      </c>
+    <row r="38" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="7"/>
       <c r="C38" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2414,10 +2439,8 @@
       <c r="AG38" s="13"/>
       <c r="AH38" s="13"/>
     </row>
-    <row r="39" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="7" t="s">
-        <v>0</v>
-      </c>
+    <row r="39" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="7"/>
       <c r="C39" s="25">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -2454,7 +2477,7 @@
       <c r="AG39" s="13"/>
       <c r="AH39" s="13"/>
     </row>
-    <row r="40" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="7"/>
       <c r="C40" s="25">
         <f t="shared" si="14"/>
@@ -2492,7 +2515,7 @@
       <c r="AG40" s="13"/>
       <c r="AH40" s="13"/>
     </row>
-    <row r="41" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="7"/>
       <c r="C41" s="25">
         <f t="shared" si="14"/>
@@ -2530,7 +2553,7 @@
       <c r="AG41" s="13"/>
       <c r="AH41" s="13"/>
     </row>
-    <row r="42" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="7"/>
       <c r="C42" s="25">
         <f t="shared" si="14"/>
@@ -2568,7 +2591,7 @@
       <c r="AG42" s="13"/>
       <c r="AH42" s="13"/>
     </row>
-    <row r="43" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="7"/>
       <c r="C43" s="25">
         <f t="shared" si="14"/>
@@ -2606,7 +2629,7 @@
       <c r="AG43" s="13"/>
       <c r="AH43" s="13"/>
     </row>
-    <row r="44" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="7"/>
       <c r="C44" s="25">
         <f t="shared" si="14"/>
@@ -2644,7 +2667,7 @@
       <c r="AG44" s="13"/>
       <c r="AH44" s="13"/>
     </row>
-    <row r="45" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="7"/>
       <c r="C45" s="25">
         <f t="shared" si="14"/>
@@ -2682,7 +2705,7 @@
       <c r="AG45" s="13"/>
       <c r="AH45" s="13"/>
     </row>
-    <row r="46" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="8"/>
       <c r="C46" s="25">
         <f t="shared" si="14"/>
@@ -2727,36 +2750,6 @@
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D11:P18 D21:P29 D19:H20 J19:P20">
-    <cfRule type="colorScale" priority="79">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:Q10 Q11:Q29">
-    <cfRule type="colorScale" priority="76">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R10:Z29">
-    <cfRule type="colorScale" priority="75">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C10">
     <cfRule type="dataBar" priority="73">
       <dataBar>
@@ -2771,634 +2764,18 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:P30">
-    <cfRule type="colorScale" priority="72">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q30">
-    <cfRule type="colorScale" priority="70">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R30:Z30">
-    <cfRule type="colorScale" priority="69">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:P35">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q31:Q35">
-    <cfRule type="colorScale" priority="66">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R31:Z35">
-    <cfRule type="colorScale" priority="65">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36:P40">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q36:Q40">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R36:Z40">
-    <cfRule type="colorScale" priority="61">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41:P41">
-    <cfRule type="colorScale" priority="60">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q41">
-    <cfRule type="colorScale" priority="58">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R41:Z41">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42:P46">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q42:Q46">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R42:Z46">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA10:AA29">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA30">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA31:AA35">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA36:AA40">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA41">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA42:AA46">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AB29">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB30">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB31:AB35">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB36:AB40">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB41">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB42:AB46">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC10:AC29">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC30">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC31:AC35">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC36:AC40">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC41">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC42:AC46">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD10:AD29">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD30">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD31:AD35">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD36:AD40">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD41">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD42:AD46">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE10:AE29">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE30">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE31:AE35">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE36:AE40">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE41">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE42:AE46">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AF29">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF30">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF31:AF35">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF36:AF40">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF41">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF42:AF46">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG10:AG29">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG30">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG31:AG35">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG36:AG40">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG41">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG42:AG46">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH10:AH29">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH30">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH31:AH35">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH36:AH40">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH41">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH42:AH46">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="C10:C46">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A2C7A50C-F572-416B-9495-8A28D149BC35}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C46">
@@ -3415,26 +2792,72 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C46">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFB628"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A2C7A50C-F572-416B-9495-8A28D149BC35}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:AH46">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
+  <conditionalFormatting sqref="D11:P18 D21:P29 D19:H20 J19:P20">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:P30">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:P35">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:P40">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41:P41">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42:P46">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:Q10 Q11:Q29">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
@@ -3451,6 +2874,606 @@
           <x14:id>{BCD65580-FCE2-4CC5-9CCE-B782BE912BFA}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:AH46">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q30">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q31:Q35">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q36:Q40">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q41">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q42:Q46">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10:Z29">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R30:Z30">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R31:Z35">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R36:Z40">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R41:Z41">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R42:Z46">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA10:AA29">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA30">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA31:AA35">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA36:AA40">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA41">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA42:AA46">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10:AB29">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB30">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB31:AB35">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB36:AB40">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB41">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB42:AB46">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC10:AC29">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC30">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC31:AC35">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC36:AC40">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC41">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC42:AC46">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD10:AD29">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD30">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD31:AD35">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD36:AD40">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD41">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD42:AD46">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE10:AE29">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE30">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE31:AE35">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE36:AE40">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE41">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE42:AE46">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10:AF29">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF30">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF31:AF35">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF36:AF40">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF41">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF42:AF46">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG10:AG29">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG30">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG31:AG35">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG36:AG40">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG41">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG42:AG46">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH10:AH29">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH30">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH31:AH35">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH36:AH40">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH41">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH42:AH46">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3472,6 +3495,17 @@
           <xm:sqref>C10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A2C7A50C-F572-416B-9495-8A28D149BC35}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C10:C46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{91046929-9F97-4C47-9B86-AC798F7EDAC7}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
@@ -3483,17 +3517,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>C11:C46</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A2C7A50C-F572-416B-9495-8A28D149BC35}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>C10:C46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BCD65580-FCE2-4CC5-9CCE-B782BE912BFA}">

</xml_diff>